<commit_message>
USER vs user ko tham chieu dc
</commit_message>
<xml_diff>
--- a/BookStore/excel/nhanvien.xlsx
+++ b/BookStore/excel/nhanvien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>MNV</t>
   </si>
@@ -32,22 +32,34 @@
     <t>dienthoai</t>
   </si>
   <si>
-    <t>ngaytao</t>
-  </si>
-  <si>
     <t>tttk</t>
   </si>
   <si>
-    <t>sffsfs</t>
-  </si>
-  <si>
-    <t>sfsf</t>
-  </si>
-  <si>
-    <t>sfsfsf</t>
-  </si>
-  <si>
-    <t>abcd</t>
+    <t>huynv</t>
+  </si>
+  <si>
+    <t>Lương Hoàng Huy</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh city</t>
+  </si>
+  <si>
+    <t>huy@gmail.com</t>
+  </si>
+  <si>
+    <t>Huỳnh Tấn Duy</t>
+  </si>
+  <si>
+    <t>duy@gmail.com</t>
+  </si>
+  <si>
+    <t>Hồ Hữu Đại</t>
+  </si>
+  <si>
+    <t>Hồ Chí Minh city</t>
+  </si>
+  <si>
+    <t>dai@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -92,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -120,15 +132,14 @@
       <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B2" s="0"/>
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>7</v>
+      </c>
       <c r="C2" t="s" s="0">
         <v>8</v>
       </c>
@@ -139,7 +150,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="n" s="0">
-        <v>224242.0</v>
+        <v>1.0212139E7</v>
       </c>
       <c r="H2" t="b" s="0">
         <v>1</v>
@@ -147,20 +158,43 @@
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>11</v>
-      </c>
+        <v>4.0</v>
+      </c>
+      <c r="B3" s="0"/>
       <c r="C3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
+      <c r="D3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
       <c r="F3" t="n" s="0">
-        <v>0.0</v>
+        <v>1231355.0</v>
       </c>
       <c r="H3" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B4" s="0"/>
+      <c r="C4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>1.1231313E7</v>
+      </c>
+      <c r="H4" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sua sql +login xiu
</commit_message>
<xml_diff>
--- a/BookStore/excel/nhanvien.xlsx
+++ b/BookStore/excel/nhanvien.xlsx
@@ -12,14 +12,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>MNV</t>
   </si>
   <si>
-    <t>username</t>
-  </si>
-  <si>
     <t>hoten</t>
   </si>
   <si>
@@ -35,25 +32,34 @@
     <t>tttk</t>
   </si>
   <si>
-    <t>vvv</t>
-  </si>
-  <si>
     <t>Nguyễn Xuân Duy</t>
   </si>
   <si>
-    <t>tpHCM</t>
-  </si>
-  <si>
-    <t>duyxxx@mmm</t>
-  </si>
-  <si>
-    <t>ssssdada</t>
+    <t>Tp HCM</t>
+  </si>
+  <si>
+    <t>duy@gmail.com</t>
+  </si>
+  <si>
+    <t>Lê Hoàng Huy</t>
+  </si>
+  <si>
+    <t>huy@gmail.com</t>
+  </si>
+  <si>
+    <t>Lương Cẩm Đào</t>
+  </si>
+  <si>
+    <t>dao@gmail.com</t>
   </si>
   <si>
     <t>Huỳnh Tấn Dương</t>
   </si>
   <si>
-    <t>sss</t>
+    <t>Đức Phổ</t>
+  </si>
+  <si>
+    <t>duong@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -98,7 +104,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -123,53 +129,84 @@
       <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
-        <v>6</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>27.0</v>
+        <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>2342342.0</v>
-      </c>
-      <c r="G2" t="b" s="0">
+      <c r="E2" t="n" s="0">
+        <v>9.4385435E7</v>
+      </c>
+      <c r="F2" t="b" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n" s="0">
-        <v>28.0</v>
+        <v>5.0</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>9.43854343E8</v>
+      </c>
+      <c r="F3" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C4" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="E4" t="n" s="0">
+        <v>4.58345663E8</v>
+      </c>
+      <c r="F4" t="b" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>123131.0</v>
-      </c>
-      <c r="G3" t="b" s="0">
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E5" t="n" s="0">
+        <v>2.4242113E7</v>
+      </c>
+      <c r="F5" t="b" s="0">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: km - ishidden, sua khach hang
</commit_message>
<xml_diff>
--- a/BookStore/excel/nhanvien.xlsx
+++ b/BookStore/excel/nhanvien.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>MNV</t>
   </si>
@@ -32,34 +32,28 @@
     <t>tttk</t>
   </si>
   <si>
-    <t>Nguyễn Xuân Duy</t>
-  </si>
-  <si>
-    <t>Tp HCM</t>
-  </si>
-  <si>
-    <t>duy@gmail.com</t>
-  </si>
-  <si>
-    <t>Lê Hoàng Huy</t>
-  </si>
-  <si>
-    <t>huy@gmail.com</t>
-  </si>
-  <si>
-    <t>Lương Cẩm Đào</t>
-  </si>
-  <si>
-    <t>dao@gmail.com</t>
-  </si>
-  <si>
-    <t>Huỳnh Tấn Dương</t>
-  </si>
-  <si>
-    <t>Đức Phổ</t>
-  </si>
-  <si>
-    <t>duong@gmail.com</t>
+    <t>dương</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>huy</t>
+  </si>
+  <si>
+    <t>179</t>
+  </si>
+  <si>
+    <t>@gmail.com</t>
+  </si>
+  <si>
+    <t>afafaf</t>
+  </si>
+  <si>
+    <t>255252sffs</t>
+  </si>
+  <si>
+    <t>ssfsfsf</t>
   </si>
 </sst>
 </file>
@@ -132,7 +126,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B2" t="s" s="0">
         <v>6</v>
@@ -141,10 +135,10 @@
         <v>7</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>9.4385435E7</v>
+        <v>1.0</v>
       </c>
       <c r="F2" t="b" s="0">
         <v>1</v>
@@ -155,16 +149,16 @@
         <v>5.0</v>
       </c>
       <c r="B3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>9</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>7</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>10</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>9.43854343E8</v>
+        <v>9.0</v>
       </c>
       <c r="F3" t="b" s="0">
         <v>1</v>
@@ -175,16 +169,16 @@
         <v>6.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>4.58345663E8</v>
+        <v>9.0</v>
       </c>
       <c r="F4" t="b" s="0">
         <v>1</v>
@@ -192,19 +186,19 @@
     </row>
     <row r="5">
       <c r="A5" t="n" s="0">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
       <c r="B5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="C5" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>15</v>
-      </c>
       <c r="E5" t="n" s="0">
-        <v>2.4242113E7</v>
+        <v>8.37002627E8</v>
       </c>
       <c r="F5" t="b" s="0">
         <v>1</v>

</xml_diff>